<commit_message>
Generalised and tested on 2 problems.
</commit_message>
<xml_diff>
--- a/excel_sheets/Toy-1D-Problem.xlsx
+++ b/excel_sheets/Toy-1D-Problem.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BillTubbs\bayes-opt-examples\excel_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF1E447-9165-4939-8607-1EE7D45FA864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E983B7AF-6963-4950-AA6B-C3A0CD820418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="397" windowWidth="27540" windowHeight="13321" xr2:uid="{0B74BFA1-2546-4EB0-A89E-EF752D6C8597}"/>
+    <workbookView xWindow="1028" yWindow="735" windowWidth="27539" windowHeight="13320" xr2:uid="{0B74BFA1-2546-4EB0-A89E-EF752D6C8597}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,15 +36,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>Toy 1D Problem</t>
+    <t>f(x)</t>
   </si>
   <si>
-    <t>x0</t>
+    <t>name</t>
   </si>
   <si>
-    <t>f(x)</t>
+    <t>x</t>
+  </si>
+  <si>
+    <t>x_lb</t>
+  </si>
+  <si>
+    <t>x_ub</t>
+  </si>
+  <si>
+    <t>Toy1DProblem</t>
   </si>
 </sst>
 </file>
@@ -437,22 +446,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{955E2372-102B-4997-A1CD-1CA94E042F50}">
-  <dimension ref="B2:C5"/>
+  <dimension ref="B2:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
         <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <f>1 / (-0.05 * $C$4 ^ 2 - COS($C$4) + 0.25 * SIN(3 * $C$4 + 0.8) + 5)</f>
+        <v>0.29041392127738885</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1">
         <v>5</v>
@@ -460,11 +481,18 @@
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="2">
-        <f>1 / (-0.05 * $C$4 ^ 2 - COS($C$4) + 0.25 * SIN(3 * $C$4 + 0.8) + 5)</f>
-        <v>0.29041392127738885</v>
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved to module and pytests.
</commit_message>
<xml_diff>
--- a/excel_sheets/Toy-1D-Problem.xlsx
+++ b/excel_sheets/Toy-1D-Problem.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BillTubbs\bayes-opt-examples\excel_sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/billtubbs/bayes-opt-examples/excel_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E022838E-6390-422E-A1E3-B07D07589ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEAA529-64CD-0940-B2A4-F4C91461FEEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1028" yWindow="735" windowWidth="27539" windowHeight="13320" xr2:uid="{0B74BFA1-2546-4EB0-A89E-EF752D6C8597}"/>
+    <workbookView xWindow="1020" yWindow="740" windowWidth="27540" windowHeight="13320" xr2:uid="{0B74BFA1-2546-4EB0-A89E-EF752D6C8597}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -452,9 +452,9 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -462,7 +462,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -471,7 +471,7 @@
         <v>0.29041392127738885</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -479,7 +479,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -487,7 +487,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>4</v>
       </c>

</xml_diff>